<commit_message>
remove the bad apple from E. coruscans and lots of other revisions
</commit_message>
<xml_diff>
--- a/Etelis snappers Migrate Hypothesis AML_EDC.xlsx
+++ b/Etelis snappers Migrate Hypothesis AML_EDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/github/Etelis_migrate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF3DC2A-5271-2944-B819-30917A84A0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342DD536-7CE7-8340-A65C-CFAC842A9201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9200" yWindow="3100" windowWidth="36560" windowHeight="23440" xr2:uid="{39C883B7-0A43-4141-AA2B-C114A9F3D6A1}"/>
+    <workbookView xWindow="9200" yWindow="3100" windowWidth="36560" windowHeight="23440" activeTab="1" xr2:uid="{39C883B7-0A43-4141-AA2B-C114A9F3D6A1}"/>
   </bookViews>
   <sheets>
     <sheet name="coruscans" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="32">
   <si>
     <t>panmixia</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Pure gene flow 1</t>
+  </si>
+  <si>
+    <t>Pure gene flow full</t>
   </si>
 </sst>
 </file>
@@ -1992,7 +1995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E9DF87-F22F-48FB-A451-9F3B436CD98F}">
   <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -3041,10 +3044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009CE635-CA86-164F-8BB5-B9F92AAA9A92}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3499,6 +3502,65 @@
         <v>2</v>
       </c>
     </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>